<commit_message>
Update maternal side of EMPDSR
</commit_message>
<xml_diff>
--- a/icd_code.xlsx
+++ b/icd_code.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elela\eclipse-workspace\olinc\pdsr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B4C3453-B6D2-47E9-B298-2305D33E766D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97AA8940-8C9F-4B4F-B128-D27567BCF546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{4E9AFF5D-8A62-4051-8A36-60E580F67420}"/>
   </bookViews>
@@ -5839,33 +5839,6 @@
     <t>icd_mmg_desc</t>
   </si>
   <si>
-    <t>G1</t>
-  </si>
-  <si>
-    <t>G2</t>
-  </si>
-  <si>
-    <t>G3</t>
-  </si>
-  <si>
-    <t>G4</t>
-  </si>
-  <si>
-    <t>G5</t>
-  </si>
-  <si>
-    <t>G6</t>
-  </si>
-  <si>
-    <t>G7</t>
-  </si>
-  <si>
-    <t>G8</t>
-  </si>
-  <si>
-    <t>G9</t>
-  </si>
-  <si>
     <t>Pregnancy with abortive outcome</t>
   </si>
   <si>
@@ -6965,6 +6938,33 @@
   </si>
   <si>
     <t>Coincidental causes</t>
+  </si>
+  <si>
+    <t>MM1</t>
+  </si>
+  <si>
+    <t>MM2</t>
+  </si>
+  <si>
+    <t>MM3</t>
+  </si>
+  <si>
+    <t>MM4</t>
+  </si>
+  <si>
+    <t>MM5</t>
+  </si>
+  <si>
+    <t>MM6</t>
+  </si>
+  <si>
+    <t>MM7</t>
+  </si>
+  <si>
+    <t>MM8</t>
+  </si>
+  <si>
+    <t>MM9</t>
   </si>
 </sst>
 </file>
@@ -7836,10 +7836,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{650E5542-A4BF-460B-879B-504B57334855}">
   <dimension ref="A1:J1129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A908" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A1103" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A939" sqref="A939"/>
-      <selection pane="topRight" activeCell="B925" sqref="B925"/>
+      <selection pane="topRight" activeCell="C1129" sqref="C1129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33333,10 +33333,10 @@
         <v>1882</v>
       </c>
       <c r="F918" t="s">
+        <v>2306</v>
+      </c>
+      <c r="J918" t="s">
         <v>1939</v>
-      </c>
-      <c r="J918" t="s">
-        <v>1948</v>
       </c>
     </row>
     <row r="919" spans="1:10" x14ac:dyDescent="0.3">
@@ -33347,10 +33347,10 @@
         <v>1883</v>
       </c>
       <c r="F919" t="s">
+        <v>2306</v>
+      </c>
+      <c r="J919" t="s">
         <v>1939</v>
-      </c>
-      <c r="J919" t="s">
-        <v>1948</v>
       </c>
     </row>
     <row r="920" spans="1:10" x14ac:dyDescent="0.3">
@@ -33361,10 +33361,10 @@
         <v>1885</v>
       </c>
       <c r="F920" t="s">
+        <v>2306</v>
+      </c>
+      <c r="J920" t="s">
         <v>1939</v>
-      </c>
-      <c r="J920" t="s">
-        <v>1948</v>
       </c>
     </row>
     <row r="921" spans="1:10" x14ac:dyDescent="0.3">
@@ -33375,10 +33375,10 @@
         <v>1886</v>
       </c>
       <c r="F921" t="s">
+        <v>2306</v>
+      </c>
+      <c r="J921" t="s">
         <v>1939</v>
-      </c>
-      <c r="J921" t="s">
-        <v>1948</v>
       </c>
     </row>
     <row r="922" spans="1:10" x14ac:dyDescent="0.3">
@@ -33389,10 +33389,10 @@
         <v>1888</v>
       </c>
       <c r="F922" t="s">
+        <v>2306</v>
+      </c>
+      <c r="J922" t="s">
         <v>1939</v>
-      </c>
-      <c r="J922" t="s">
-        <v>1948</v>
       </c>
     </row>
     <row r="923" spans="1:10" x14ac:dyDescent="0.3">
@@ -33403,10 +33403,10 @@
         <v>1890</v>
       </c>
       <c r="F923" t="s">
+        <v>2306</v>
+      </c>
+      <c r="J923" t="s">
         <v>1939</v>
-      </c>
-      <c r="J923" t="s">
-        <v>1948</v>
       </c>
     </row>
     <row r="924" spans="1:10" x14ac:dyDescent="0.3">
@@ -33417,10 +33417,10 @@
         <v>1893</v>
       </c>
       <c r="F924" t="s">
+        <v>2306</v>
+      </c>
+      <c r="J924" t="s">
         <v>1939</v>
-      </c>
-      <c r="J924" t="s">
-        <v>1948</v>
       </c>
     </row>
     <row r="925" spans="1:10" x14ac:dyDescent="0.3">
@@ -33431,10 +33431,10 @@
         <v>1894</v>
       </c>
       <c r="F925" t="s">
+        <v>2306</v>
+      </c>
+      <c r="J925" t="s">
         <v>1939</v>
-      </c>
-      <c r="J925" t="s">
-        <v>1948</v>
       </c>
     </row>
     <row r="926" spans="1:10" x14ac:dyDescent="0.3">
@@ -33445,10 +33445,10 @@
         <v>1895</v>
       </c>
       <c r="F926" t="s">
+        <v>2306</v>
+      </c>
+      <c r="J926" t="s">
         <v>1939</v>
-      </c>
-      <c r="J926" t="s">
-        <v>1948</v>
       </c>
     </row>
     <row r="927" spans="1:10" x14ac:dyDescent="0.3">
@@ -33459,10 +33459,10 @@
         <v>1896</v>
       </c>
       <c r="F927" t="s">
+        <v>2306</v>
+      </c>
+      <c r="J927" t="s">
         <v>1939</v>
-      </c>
-      <c r="J927" t="s">
-        <v>1948</v>
       </c>
     </row>
     <row r="928" spans="1:10" x14ac:dyDescent="0.3">
@@ -33473,10 +33473,10 @@
         <v>1898</v>
       </c>
       <c r="F928" t="s">
+        <v>2306</v>
+      </c>
+      <c r="J928" t="s">
         <v>1939</v>
-      </c>
-      <c r="J928" t="s">
-        <v>1948</v>
       </c>
     </row>
     <row r="929" spans="1:10" x14ac:dyDescent="0.3">
@@ -33487,10 +33487,10 @@
         <v>1900</v>
       </c>
       <c r="F929" t="s">
+        <v>2306</v>
+      </c>
+      <c r="J929" t="s">
         <v>1939</v>
-      </c>
-      <c r="J929" t="s">
-        <v>1948</v>
       </c>
     </row>
     <row r="930" spans="1:10" x14ac:dyDescent="0.3">
@@ -33501,10 +33501,10 @@
         <v>1902</v>
       </c>
       <c r="F930" t="s">
+        <v>2306</v>
+      </c>
+      <c r="J930" t="s">
         <v>1939</v>
-      </c>
-      <c r="J930" t="s">
-        <v>1948</v>
       </c>
     </row>
     <row r="931" spans="1:10" x14ac:dyDescent="0.3">
@@ -33515,10 +33515,10 @@
         <v>1904</v>
       </c>
       <c r="F931" t="s">
+        <v>2306</v>
+      </c>
+      <c r="J931" t="s">
         <v>1939</v>
-      </c>
-      <c r="J931" t="s">
-        <v>1948</v>
       </c>
     </row>
     <row r="932" spans="1:10" x14ac:dyDescent="0.3">
@@ -33529,10 +33529,10 @@
         <v>1906</v>
       </c>
       <c r="F932" t="s">
+        <v>2306</v>
+      </c>
+      <c r="J932" t="s">
         <v>1939</v>
-      </c>
-      <c r="J932" t="s">
-        <v>1948</v>
       </c>
     </row>
     <row r="933" spans="1:10" x14ac:dyDescent="0.3">
@@ -33543,10 +33543,10 @@
         <v>1908</v>
       </c>
       <c r="F933" t="s">
+        <v>2306</v>
+      </c>
+      <c r="J933" t="s">
         <v>1939</v>
-      </c>
-      <c r="J933" t="s">
-        <v>1948</v>
       </c>
     </row>
     <row r="934" spans="1:10" x14ac:dyDescent="0.3">
@@ -33557,10 +33557,10 @@
         <v>1910</v>
       </c>
       <c r="F934" t="s">
+        <v>2306</v>
+      </c>
+      <c r="J934" t="s">
         <v>1939</v>
-      </c>
-      <c r="J934" t="s">
-        <v>1948</v>
       </c>
     </row>
     <row r="935" spans="1:10" x14ac:dyDescent="0.3">
@@ -33571,10 +33571,10 @@
         <v>1912</v>
       </c>
       <c r="F935" t="s">
+        <v>2306</v>
+      </c>
+      <c r="J935" t="s">
         <v>1939</v>
-      </c>
-      <c r="J935" t="s">
-        <v>1948</v>
       </c>
     </row>
     <row r="936" spans="1:10" x14ac:dyDescent="0.3">
@@ -33585,10 +33585,10 @@
         <v>1914</v>
       </c>
       <c r="F936" t="s">
+        <v>2306</v>
+      </c>
+      <c r="J936" t="s">
         <v>1939</v>
-      </c>
-      <c r="J936" t="s">
-        <v>1948</v>
       </c>
     </row>
     <row r="937" spans="1:10" x14ac:dyDescent="0.3">
@@ -33599,10 +33599,10 @@
         <v>1916</v>
       </c>
       <c r="F937" t="s">
+        <v>2306</v>
+      </c>
+      <c r="J937" t="s">
         <v>1939</v>
-      </c>
-      <c r="J937" t="s">
-        <v>1948</v>
       </c>
     </row>
     <row r="938" spans="1:10" x14ac:dyDescent="0.3">
@@ -33613,10 +33613,10 @@
         <v>1918</v>
       </c>
       <c r="F938" t="s">
+        <v>2306</v>
+      </c>
+      <c r="J938" t="s">
         <v>1939</v>
-      </c>
-      <c r="J938" t="s">
-        <v>1948</v>
       </c>
     </row>
     <row r="939" spans="1:10" x14ac:dyDescent="0.3">
@@ -33627,10 +33627,10 @@
         <v>1920</v>
       </c>
       <c r="F939" t="s">
+        <v>2306</v>
+      </c>
+      <c r="J939" t="s">
         <v>1939</v>
-      </c>
-      <c r="J939" t="s">
-        <v>1948</v>
       </c>
     </row>
     <row r="940" spans="1:10" x14ac:dyDescent="0.3">
@@ -33641,10 +33641,10 @@
         <v>1922</v>
       </c>
       <c r="F940" t="s">
+        <v>2306</v>
+      </c>
+      <c r="J940" t="s">
         <v>1939</v>
-      </c>
-      <c r="J940" t="s">
-        <v>1948</v>
       </c>
     </row>
     <row r="941" spans="1:10" x14ac:dyDescent="0.3">
@@ -33655,10 +33655,10 @@
         <v>1923</v>
       </c>
       <c r="F941" t="s">
+        <v>2306</v>
+      </c>
+      <c r="J941" t="s">
         <v>1939</v>
-      </c>
-      <c r="J941" t="s">
-        <v>1948</v>
       </c>
     </row>
     <row r="942" spans="1:10" x14ac:dyDescent="0.3">
@@ -33669,10 +33669,10 @@
         <v>1926</v>
       </c>
       <c r="F942" t="s">
+        <v>2306</v>
+      </c>
+      <c r="J942" t="s">
         <v>1939</v>
-      </c>
-      <c r="J942" t="s">
-        <v>1948</v>
       </c>
     </row>
     <row r="943" spans="1:10" x14ac:dyDescent="0.3">
@@ -33683,10 +33683,10 @@
         <v>1928</v>
       </c>
       <c r="F943" t="s">
+        <v>2306</v>
+      </c>
+      <c r="J943" t="s">
         <v>1939</v>
-      </c>
-      <c r="J943" t="s">
-        <v>1948</v>
       </c>
     </row>
     <row r="944" spans="1:10" x14ac:dyDescent="0.3">
@@ -33697,10 +33697,10 @@
         <v>1930</v>
       </c>
       <c r="F944" t="s">
+        <v>2306</v>
+      </c>
+      <c r="J944" t="s">
         <v>1939</v>
-      </c>
-      <c r="J944" t="s">
-        <v>1948</v>
       </c>
     </row>
     <row r="945" spans="1:10" x14ac:dyDescent="0.3">
@@ -33711,10 +33711,10 @@
         <v>1932</v>
       </c>
       <c r="F945" t="s">
+        <v>2306</v>
+      </c>
+      <c r="J945" t="s">
         <v>1939</v>
-      </c>
-      <c r="J945" t="s">
-        <v>1948</v>
       </c>
     </row>
     <row r="946" spans="1:10" x14ac:dyDescent="0.3">
@@ -33725,10 +33725,10 @@
         <v>1934</v>
       </c>
       <c r="F946" t="s">
+        <v>2306</v>
+      </c>
+      <c r="J946" t="s">
         <v>1939</v>
-      </c>
-      <c r="J946" t="s">
-        <v>1948</v>
       </c>
     </row>
     <row r="947" spans="1:10" x14ac:dyDescent="0.3">
@@ -33739,2558 +33739,2558 @@
         <v>1936</v>
       </c>
       <c r="F947" t="s">
+        <v>2306</v>
+      </c>
+      <c r="J947" t="s">
         <v>1939</v>
-      </c>
-      <c r="J947" t="s">
-        <v>1948</v>
       </c>
     </row>
     <row r="948" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A948" t="s">
-        <v>1949</v>
+        <v>1940</v>
       </c>
       <c r="B948" t="s">
-        <v>1950</v>
+        <v>1941</v>
       </c>
       <c r="F948" t="s">
-        <v>1940</v>
+        <v>2307</v>
       </c>
       <c r="J948" s="1" t="s">
-        <v>2307</v>
+        <v>2298</v>
       </c>
     </row>
     <row r="949" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A949" t="s">
-        <v>1952</v>
+        <v>1943</v>
       </c>
       <c r="B949" t="s">
-        <v>1951</v>
+        <v>1942</v>
       </c>
       <c r="F949" t="s">
-        <v>1940</v>
+        <v>2307</v>
       </c>
       <c r="J949" s="1" t="s">
-        <v>2307</v>
+        <v>2298</v>
       </c>
     </row>
     <row r="950" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A950" t="s">
-        <v>1956</v>
+        <v>1947</v>
       </c>
       <c r="B950" t="s">
-        <v>1953</v>
+        <v>1944</v>
       </c>
       <c r="F950" t="s">
-        <v>1940</v>
+        <v>2307</v>
       </c>
       <c r="J950" s="1" t="s">
-        <v>2307</v>
+        <v>2298</v>
       </c>
     </row>
     <row r="951" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A951" t="s">
-        <v>1957</v>
+        <v>1948</v>
       </c>
       <c r="B951" t="s">
-        <v>1954</v>
+        <v>1945</v>
       </c>
       <c r="F951" t="s">
-        <v>1940</v>
+        <v>2307</v>
       </c>
       <c r="J951" s="1" t="s">
-        <v>2307</v>
+        <v>2298</v>
       </c>
     </row>
     <row r="952" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A952" t="s">
-        <v>1958</v>
+        <v>1949</v>
       </c>
       <c r="B952" t="s">
-        <v>1955</v>
+        <v>1946</v>
       </c>
       <c r="F952" t="s">
-        <v>1940</v>
+        <v>2307</v>
       </c>
       <c r="J952" s="1" t="s">
-        <v>2307</v>
+        <v>2298</v>
       </c>
     </row>
     <row r="953" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A953" t="s">
-        <v>1959</v>
+        <v>1950</v>
       </c>
       <c r="B953" t="s">
-        <v>1960</v>
+        <v>1951</v>
       </c>
       <c r="F953" t="s">
-        <v>1940</v>
+        <v>2307</v>
       </c>
       <c r="J953" s="1" t="s">
-        <v>2307</v>
+        <v>2298</v>
       </c>
     </row>
     <row r="954" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A954" t="s">
-        <v>1961</v>
+        <v>1952</v>
       </c>
       <c r="B954" t="s">
-        <v>1966</v>
+        <v>1957</v>
       </c>
       <c r="F954" t="s">
-        <v>1940</v>
+        <v>2307</v>
       </c>
       <c r="J954" s="1" t="s">
-        <v>2307</v>
+        <v>2298</v>
       </c>
     </row>
     <row r="955" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A955" t="s">
-        <v>1962</v>
+        <v>1953</v>
       </c>
       <c r="B955" t="s">
-        <v>1967</v>
+        <v>1958</v>
       </c>
       <c r="F955" t="s">
-        <v>1940</v>
+        <v>2307</v>
       </c>
       <c r="J955" s="1" t="s">
-        <v>2307</v>
+        <v>2298</v>
       </c>
     </row>
     <row r="956" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A956" t="s">
-        <v>1963</v>
+        <v>1954</v>
       </c>
       <c r="B956" t="s">
-        <v>1968</v>
+        <v>1959</v>
       </c>
       <c r="F956" t="s">
-        <v>1940</v>
+        <v>2307</v>
       </c>
       <c r="J956" s="1" t="s">
-        <v>2307</v>
+        <v>2298</v>
       </c>
     </row>
     <row r="957" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A957" t="s">
-        <v>1964</v>
+        <v>1955</v>
       </c>
       <c r="B957" t="s">
-        <v>1969</v>
+        <v>1960</v>
       </c>
       <c r="F957" t="s">
-        <v>1940</v>
+        <v>2307</v>
       </c>
       <c r="J957" s="1" t="s">
-        <v>2307</v>
+        <v>2298</v>
       </c>
     </row>
     <row r="958" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A958" t="s">
-        <v>1965</v>
+        <v>1956</v>
       </c>
       <c r="B958" t="s">
-        <v>1970</v>
+        <v>1961</v>
       </c>
       <c r="F958" t="s">
-        <v>1940</v>
+        <v>2307</v>
       </c>
       <c r="J958" s="1" t="s">
-        <v>2307</v>
+        <v>2298</v>
       </c>
     </row>
     <row r="959" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A959" t="s">
-        <v>1971</v>
+        <v>1962</v>
       </c>
       <c r="B959" t="s">
-        <v>1972</v>
+        <v>1963</v>
       </c>
       <c r="F959" t="s">
-        <v>1940</v>
+        <v>2307</v>
       </c>
       <c r="J959" s="1" t="s">
-        <v>2307</v>
+        <v>2298</v>
       </c>
     </row>
     <row r="960" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A960" t="s">
-        <v>1977</v>
+        <v>1968</v>
       </c>
       <c r="B960" t="s">
-        <v>1973</v>
+        <v>1964</v>
       </c>
       <c r="F960" t="s">
-        <v>1940</v>
+        <v>2307</v>
       </c>
       <c r="J960" s="1" t="s">
-        <v>2307</v>
+        <v>2298</v>
       </c>
     </row>
     <row r="961" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A961" t="s">
-        <v>1978</v>
+        <v>1969</v>
       </c>
       <c r="B961" t="s">
-        <v>1974</v>
+        <v>1965</v>
       </c>
       <c r="F961" t="s">
-        <v>1940</v>
+        <v>2307</v>
       </c>
       <c r="J961" s="1" t="s">
-        <v>2307</v>
+        <v>2298</v>
       </c>
     </row>
     <row r="962" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A962" t="s">
-        <v>1979</v>
+        <v>1970</v>
       </c>
       <c r="B962" t="s">
-        <v>1975</v>
+        <v>1966</v>
       </c>
       <c r="F962" t="s">
-        <v>1940</v>
+        <v>2307</v>
       </c>
       <c r="J962" s="1" t="s">
-        <v>2307</v>
+        <v>2298</v>
       </c>
     </row>
     <row r="963" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A963" t="s">
-        <v>1980</v>
+        <v>1971</v>
       </c>
       <c r="B963" t="s">
-        <v>1976</v>
+        <v>1967</v>
       </c>
       <c r="F963" t="s">
-        <v>1940</v>
+        <v>2307</v>
       </c>
       <c r="J963" s="1" t="s">
-        <v>2307</v>
+        <v>2298</v>
       </c>
     </row>
     <row r="964" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A964" t="s">
-        <v>1981</v>
+        <v>1972</v>
       </c>
       <c r="B964" t="s">
-        <v>1982</v>
+        <v>1973</v>
       </c>
       <c r="F964" t="s">
-        <v>1940</v>
+        <v>2307</v>
       </c>
       <c r="J964" s="1" t="s">
-        <v>2307</v>
+        <v>2298</v>
       </c>
     </row>
     <row r="965" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A965" t="s">
-        <v>1983</v>
+        <v>1974</v>
       </c>
       <c r="B965" t="s">
-        <v>1984</v>
+        <v>1975</v>
       </c>
       <c r="F965" t="s">
-        <v>1941</v>
+        <v>2308</v>
       </c>
       <c r="J965" s="1" t="s">
-        <v>2308</v>
+        <v>2299</v>
       </c>
     </row>
     <row r="966" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A966" t="s">
-        <v>1988</v>
+        <v>1979</v>
       </c>
       <c r="B966" t="s">
-        <v>1985</v>
+        <v>1976</v>
       </c>
       <c r="F966" t="s">
-        <v>1941</v>
+        <v>2308</v>
       </c>
       <c r="J966" s="1" t="s">
-        <v>2308</v>
+        <v>2299</v>
       </c>
     </row>
     <row r="967" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A967" t="s">
-        <v>1989</v>
+        <v>1980</v>
       </c>
       <c r="B967" t="s">
-        <v>1986</v>
+        <v>1977</v>
       </c>
       <c r="F967" t="s">
-        <v>1941</v>
+        <v>2308</v>
       </c>
       <c r="J967" s="1" t="s">
-        <v>2308</v>
+        <v>2299</v>
       </c>
     </row>
     <row r="968" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A968" t="s">
-        <v>1990</v>
+        <v>1981</v>
       </c>
       <c r="B968" t="s">
-        <v>1987</v>
+        <v>1978</v>
       </c>
       <c r="F968" t="s">
-        <v>1941</v>
+        <v>2308</v>
       </c>
       <c r="J968" s="1" t="s">
-        <v>2308</v>
+        <v>2299</v>
       </c>
     </row>
     <row r="969" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A969" t="s">
-        <v>1991</v>
+        <v>1982</v>
       </c>
       <c r="B969" t="s">
-        <v>1992</v>
+        <v>1983</v>
       </c>
       <c r="F969" t="s">
-        <v>1941</v>
+        <v>2308</v>
       </c>
       <c r="J969" s="1" t="s">
-        <v>2308</v>
+        <v>2299</v>
       </c>
     </row>
     <row r="970" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A970" t="s">
-        <v>1993</v>
+        <v>1984</v>
       </c>
       <c r="B970" t="s">
-        <v>1994</v>
+        <v>1985</v>
       </c>
       <c r="F970" t="s">
-        <v>1941</v>
+        <v>2308</v>
       </c>
       <c r="J970" s="1" t="s">
-        <v>2308</v>
+        <v>2299</v>
       </c>
     </row>
     <row r="971" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A971" t="s">
-        <v>1995</v>
+        <v>1986</v>
       </c>
       <c r="B971" t="s">
-        <v>2001</v>
+        <v>1992</v>
       </c>
       <c r="F971" t="s">
-        <v>1941</v>
+        <v>2308</v>
       </c>
       <c r="J971" s="1" t="s">
-        <v>2308</v>
+        <v>2299</v>
       </c>
     </row>
     <row r="972" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A972" t="s">
-        <v>1996</v>
+        <v>1987</v>
       </c>
       <c r="B972" t="s">
-        <v>2002</v>
+        <v>1993</v>
       </c>
       <c r="F972" t="s">
-        <v>1941</v>
+        <v>2308</v>
       </c>
       <c r="J972" s="1" t="s">
-        <v>2308</v>
+        <v>2299</v>
       </c>
     </row>
     <row r="973" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A973" t="s">
-        <v>1997</v>
+        <v>1988</v>
       </c>
       <c r="B973" t="s">
-        <v>2003</v>
+        <v>1994</v>
       </c>
       <c r="F973" t="s">
-        <v>1941</v>
+        <v>2308</v>
       </c>
       <c r="J973" s="1" t="s">
-        <v>2308</v>
+        <v>2299</v>
       </c>
     </row>
     <row r="974" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A974" t="s">
-        <v>1998</v>
+        <v>1989</v>
       </c>
       <c r="B974" t="s">
-        <v>2004</v>
+        <v>1995</v>
       </c>
       <c r="F974" t="s">
-        <v>1941</v>
+        <v>2308</v>
       </c>
       <c r="J974" s="1" t="s">
-        <v>2308</v>
+        <v>2299</v>
       </c>
     </row>
     <row r="975" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A975" t="s">
-        <v>1999</v>
+        <v>1990</v>
       </c>
       <c r="B975" t="s">
-        <v>2005</v>
+        <v>1996</v>
       </c>
       <c r="F975" t="s">
-        <v>1941</v>
+        <v>2308</v>
       </c>
       <c r="J975" s="1" t="s">
-        <v>2308</v>
+        <v>2299</v>
       </c>
     </row>
     <row r="976" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A976" t="s">
-        <v>2000</v>
+        <v>1991</v>
       </c>
       <c r="B976" t="s">
-        <v>2006</v>
+        <v>1997</v>
       </c>
       <c r="F976" t="s">
-        <v>1941</v>
+        <v>2308</v>
       </c>
       <c r="J976" s="1" t="s">
-        <v>2308</v>
+        <v>2299</v>
       </c>
     </row>
     <row r="977" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A977" t="s">
-        <v>2007</v>
+        <v>1998</v>
       </c>
       <c r="B977" t="s">
-        <v>2011</v>
+        <v>2002</v>
       </c>
       <c r="F977" t="s">
-        <v>1941</v>
+        <v>2308</v>
       </c>
       <c r="J977" s="1" t="s">
-        <v>2308</v>
+        <v>2299</v>
       </c>
     </row>
     <row r="978" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A978" t="s">
-        <v>2008</v>
+        <v>1999</v>
       </c>
       <c r="B978" t="s">
-        <v>2011</v>
+        <v>2002</v>
       </c>
       <c r="F978" t="s">
-        <v>1941</v>
+        <v>2308</v>
       </c>
       <c r="J978" s="1" t="s">
-        <v>2308</v>
+        <v>2299</v>
       </c>
     </row>
     <row r="979" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A979" t="s">
-        <v>2009</v>
+        <v>2000</v>
       </c>
       <c r="B979" t="s">
-        <v>2012</v>
+        <v>2003</v>
       </c>
       <c r="F979" t="s">
-        <v>1941</v>
+        <v>2308</v>
       </c>
       <c r="J979" s="1" t="s">
-        <v>2308</v>
+        <v>2299</v>
       </c>
     </row>
     <row r="980" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A980" t="s">
-        <v>2010</v>
+        <v>2001</v>
       </c>
       <c r="B980" t="s">
-        <v>2013</v>
+        <v>2004</v>
       </c>
       <c r="F980" t="s">
-        <v>1941</v>
+        <v>2308</v>
       </c>
       <c r="J980" s="1" t="s">
-        <v>2308</v>
+        <v>2299</v>
       </c>
     </row>
     <row r="981" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A981" t="s">
-        <v>2014</v>
+        <v>2005</v>
       </c>
       <c r="B981" t="s">
-        <v>2015</v>
+        <v>2006</v>
       </c>
       <c r="F981" t="s">
-        <v>1941</v>
+        <v>2308</v>
       </c>
       <c r="J981" s="1" t="s">
-        <v>2308</v>
+        <v>2299</v>
       </c>
     </row>
     <row r="982" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A982" t="s">
-        <v>2019</v>
+        <v>2010</v>
       </c>
       <c r="B982" t="s">
-        <v>2016</v>
+        <v>2007</v>
       </c>
       <c r="F982" t="s">
-        <v>1941</v>
+        <v>2308</v>
       </c>
       <c r="J982" s="1" t="s">
-        <v>2308</v>
+        <v>2299</v>
       </c>
     </row>
     <row r="983" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A983" t="s">
-        <v>2020</v>
+        <v>2011</v>
       </c>
       <c r="B983" t="s">
-        <v>2017</v>
+        <v>2008</v>
       </c>
       <c r="F983" t="s">
-        <v>1941</v>
+        <v>2308</v>
       </c>
       <c r="J983" s="1" t="s">
-        <v>2308</v>
+        <v>2299</v>
       </c>
     </row>
     <row r="984" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A984" t="s">
-        <v>2021</v>
+        <v>2012</v>
       </c>
       <c r="B984" t="s">
-        <v>2018</v>
+        <v>2009</v>
       </c>
       <c r="F984" t="s">
-        <v>1941</v>
+        <v>2308</v>
       </c>
       <c r="J984" s="1" t="s">
-        <v>2308</v>
+        <v>2299</v>
       </c>
     </row>
     <row r="985" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A985" t="s">
-        <v>2022</v>
+        <v>2013</v>
       </c>
       <c r="B985" t="s">
-        <v>2023</v>
+        <v>2014</v>
       </c>
       <c r="F985" t="s">
-        <v>1941</v>
+        <v>2308</v>
       </c>
       <c r="J985" s="1" t="s">
-        <v>2308</v>
+        <v>2299</v>
       </c>
     </row>
     <row r="986" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A986" t="s">
-        <v>2024</v>
+        <v>2015</v>
       </c>
       <c r="B986" t="s">
-        <v>2029</v>
+        <v>2020</v>
       </c>
       <c r="F986" t="s">
-        <v>1941</v>
+        <v>2308</v>
       </c>
       <c r="J986" s="1" t="s">
-        <v>2308</v>
+        <v>2299</v>
       </c>
     </row>
     <row r="987" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A987" t="s">
-        <v>2025</v>
+        <v>2016</v>
       </c>
       <c r="B987" t="s">
-        <v>2030</v>
+        <v>2021</v>
       </c>
       <c r="F987" t="s">
-        <v>1941</v>
+        <v>2308</v>
       </c>
       <c r="J987" s="1" t="s">
-        <v>2308</v>
+        <v>2299</v>
       </c>
     </row>
     <row r="988" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A988" t="s">
-        <v>2026</v>
+        <v>2017</v>
       </c>
       <c r="B988" t="s">
-        <v>2031</v>
+        <v>2022</v>
       </c>
       <c r="F988" t="s">
-        <v>1941</v>
+        <v>2308</v>
       </c>
       <c r="J988" s="1" t="s">
-        <v>2308</v>
+        <v>2299</v>
       </c>
     </row>
     <row r="989" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A989" t="s">
-        <v>2027</v>
+        <v>2018</v>
       </c>
       <c r="B989" t="s">
-        <v>2032</v>
+        <v>2023</v>
       </c>
       <c r="F989" t="s">
-        <v>1941</v>
+        <v>2308</v>
       </c>
       <c r="J989" s="1" t="s">
-        <v>2308</v>
+        <v>2299</v>
       </c>
     </row>
     <row r="990" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A990" t="s">
-        <v>2028</v>
+        <v>2019</v>
       </c>
       <c r="B990" t="s">
-        <v>2033</v>
+        <v>2024</v>
       </c>
       <c r="F990" t="s">
-        <v>1941</v>
+        <v>2308</v>
       </c>
       <c r="J990" s="1" t="s">
-        <v>2308</v>
+        <v>2299</v>
       </c>
     </row>
     <row r="991" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A991" t="s">
-        <v>2034</v>
+        <v>2025</v>
       </c>
       <c r="B991" t="s">
-        <v>2035</v>
+        <v>2026</v>
       </c>
       <c r="F991" t="s">
-        <v>1941</v>
+        <v>2308</v>
       </c>
       <c r="J991" s="1" t="s">
-        <v>2308</v>
+        <v>2299</v>
       </c>
     </row>
     <row r="992" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A992" t="s">
-        <v>2036</v>
+        <v>2027</v>
       </c>
       <c r="B992" t="s">
-        <v>2037</v>
+        <v>2028</v>
       </c>
       <c r="F992" t="s">
-        <v>1941</v>
+        <v>2308</v>
       </c>
       <c r="J992" s="1" t="s">
-        <v>2308</v>
+        <v>2299</v>
       </c>
     </row>
     <row r="993" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A993" t="s">
-        <v>2038</v>
+        <v>2029</v>
       </c>
       <c r="B993" t="s">
-        <v>2039</v>
+        <v>2030</v>
       </c>
       <c r="F993" t="s">
-        <v>1941</v>
+        <v>2308</v>
       </c>
       <c r="J993" s="1" t="s">
-        <v>2308</v>
+        <v>2299</v>
       </c>
     </row>
     <row r="994" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A994" t="s">
-        <v>2040</v>
+        <v>2031</v>
       </c>
       <c r="B994" t="s">
-        <v>2041</v>
+        <v>2032</v>
       </c>
       <c r="F994" t="s">
-        <v>1941</v>
+        <v>2308</v>
       </c>
       <c r="J994" s="1" t="s">
-        <v>2308</v>
+        <v>2299</v>
       </c>
     </row>
     <row r="995" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A995" t="s">
-        <v>2042</v>
+        <v>2033</v>
       </c>
       <c r="B995" t="s">
-        <v>2043</v>
+        <v>2034</v>
       </c>
       <c r="F995" t="s">
-        <v>1941</v>
+        <v>2308</v>
       </c>
       <c r="J995" s="1" t="s">
-        <v>2308</v>
+        <v>2299</v>
       </c>
     </row>
     <row r="996" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A996" t="s">
-        <v>2044</v>
+        <v>2035</v>
       </c>
       <c r="B996" t="s">
-        <v>2052</v>
+        <v>2043</v>
       </c>
       <c r="F996" t="s">
-        <v>1942</v>
+        <v>2309</v>
       </c>
       <c r="J996" s="1" t="s">
-        <v>2309</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="997" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A997" t="s">
-        <v>2045</v>
+        <v>2036</v>
       </c>
       <c r="B997" t="s">
-        <v>2053</v>
+        <v>2044</v>
       </c>
       <c r="F997" t="s">
-        <v>1942</v>
+        <v>2309</v>
       </c>
       <c r="J997" s="1" t="s">
-        <v>2309</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="998" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A998" t="s">
-        <v>2046</v>
+        <v>2037</v>
       </c>
       <c r="B998" t="s">
-        <v>2054</v>
+        <v>2045</v>
       </c>
       <c r="F998" t="s">
-        <v>1942</v>
+        <v>2309</v>
       </c>
       <c r="J998" s="1" t="s">
-        <v>2309</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="999" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A999" t="s">
-        <v>2047</v>
+        <v>2038</v>
       </c>
       <c r="B999" t="s">
-        <v>2055</v>
+        <v>2046</v>
       </c>
       <c r="F999" t="s">
-        <v>1942</v>
+        <v>2309</v>
       </c>
       <c r="J999" s="1" t="s">
-        <v>2309</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="1000" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1000" t="s">
-        <v>2048</v>
+        <v>2039</v>
       </c>
       <c r="B1000" t="s">
-        <v>2056</v>
+        <v>2047</v>
       </c>
       <c r="F1000" t="s">
-        <v>1942</v>
+        <v>2309</v>
       </c>
       <c r="J1000" s="1" t="s">
-        <v>2309</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="1001" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1001" t="s">
-        <v>2049</v>
+        <v>2040</v>
       </c>
       <c r="B1001" t="s">
-        <v>2057</v>
+        <v>2048</v>
       </c>
       <c r="F1001" t="s">
-        <v>1942</v>
+        <v>2309</v>
       </c>
       <c r="J1001" s="1" t="s">
-        <v>2309</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="1002" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1002" t="s">
-        <v>2050</v>
+        <v>2041</v>
       </c>
       <c r="B1002" t="s">
-        <v>2058</v>
+        <v>2049</v>
       </c>
       <c r="F1002" t="s">
-        <v>1942</v>
+        <v>2309</v>
       </c>
       <c r="J1002" s="1" t="s">
-        <v>2309</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="1003" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1003" t="s">
-        <v>2051</v>
+        <v>2042</v>
       </c>
       <c r="B1003" t="s">
-        <v>2059</v>
+        <v>2050</v>
       </c>
       <c r="F1003" t="s">
-        <v>1942</v>
+        <v>2309</v>
       </c>
       <c r="J1003" s="1" t="s">
-        <v>2309</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="1004" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1004" t="s">
-        <v>2060</v>
+        <v>2051</v>
       </c>
       <c r="B1004" t="s">
-        <v>2062</v>
+        <v>2053</v>
       </c>
       <c r="F1004" t="s">
-        <v>1942</v>
+        <v>2309</v>
       </c>
       <c r="J1004" s="1" t="s">
-        <v>2309</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="1005" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1005" t="s">
-        <v>2061</v>
+        <v>2052</v>
       </c>
       <c r="B1005" t="s">
-        <v>2063</v>
+        <v>2054</v>
       </c>
       <c r="F1005" t="s">
-        <v>1942</v>
+        <v>2309</v>
       </c>
       <c r="J1005" s="1" t="s">
-        <v>2309</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="1006" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1006" t="s">
-        <v>2064</v>
+        <v>2055</v>
       </c>
       <c r="B1006" t="s">
-        <v>2065</v>
+        <v>2056</v>
       </c>
       <c r="F1006" t="s">
-        <v>1942</v>
+        <v>2309</v>
       </c>
       <c r="J1006" s="1" t="s">
-        <v>2309</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="1007" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1007" t="s">
-        <v>2066</v>
+        <v>2057</v>
       </c>
       <c r="B1007" t="s">
-        <v>2067</v>
+        <v>2058</v>
       </c>
       <c r="F1007" t="s">
-        <v>1942</v>
+        <v>2309</v>
       </c>
       <c r="J1007" s="1" t="s">
-        <v>2309</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="1008" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1008" t="s">
-        <v>2068</v>
+        <v>2059</v>
       </c>
       <c r="B1008" t="s">
-        <v>2069</v>
+        <v>2060</v>
       </c>
       <c r="F1008" t="s">
-        <v>1942</v>
+        <v>2309</v>
       </c>
       <c r="J1008" s="1" t="s">
-        <v>2309</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="1009" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1009" t="s">
-        <v>2070</v>
+        <v>2061</v>
       </c>
       <c r="B1009" t="s">
-        <v>2075</v>
+        <v>2066</v>
       </c>
       <c r="F1009" t="s">
-        <v>1942</v>
+        <v>2309</v>
       </c>
       <c r="J1009" s="1" t="s">
-        <v>2309</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="1010" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1010" t="s">
-        <v>2071</v>
+        <v>2062</v>
       </c>
       <c r="B1010" t="s">
-        <v>2076</v>
+        <v>2067</v>
       </c>
       <c r="F1010" t="s">
-        <v>1942</v>
+        <v>2309</v>
       </c>
       <c r="J1010" s="1" t="s">
-        <v>2309</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="1011" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1011" t="s">
-        <v>2072</v>
+        <v>2063</v>
       </c>
       <c r="B1011" t="s">
-        <v>2077</v>
+        <v>2068</v>
       </c>
       <c r="F1011" t="s">
-        <v>1942</v>
+        <v>2309</v>
       </c>
       <c r="J1011" s="1" t="s">
-        <v>2309</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="1012" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1012" t="s">
-        <v>2073</v>
+        <v>2064</v>
       </c>
       <c r="B1012" t="s">
-        <v>2078</v>
+        <v>2069</v>
       </c>
       <c r="F1012" t="s">
-        <v>1942</v>
+        <v>2309</v>
       </c>
       <c r="J1012" s="1" t="s">
-        <v>2309</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="1013" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1013" t="s">
-        <v>2074</v>
+        <v>2065</v>
       </c>
       <c r="B1013" t="s">
-        <v>2079</v>
+        <v>2070</v>
       </c>
       <c r="F1013" t="s">
-        <v>1942</v>
+        <v>2309</v>
       </c>
       <c r="J1013" s="1" t="s">
-        <v>2309</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="1014" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1014" t="s">
-        <v>2080</v>
+        <v>2071</v>
       </c>
       <c r="B1014" t="s">
-        <v>2084</v>
+        <v>2075</v>
       </c>
       <c r="F1014" t="s">
-        <v>1942</v>
+        <v>2309</v>
       </c>
       <c r="J1014" s="1" t="s">
-        <v>2309</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="1015" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1015" t="s">
-        <v>2081</v>
+        <v>2072</v>
       </c>
       <c r="B1015" t="s">
-        <v>2085</v>
+        <v>2076</v>
       </c>
       <c r="F1015" t="s">
-        <v>1942</v>
+        <v>2309</v>
       </c>
       <c r="J1015" s="1" t="s">
-        <v>2309</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="1016" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1016" t="s">
-        <v>2082</v>
+        <v>2073</v>
       </c>
       <c r="B1016" t="s">
-        <v>2086</v>
+        <v>2077</v>
       </c>
       <c r="F1016" t="s">
-        <v>1942</v>
+        <v>2309</v>
       </c>
       <c r="J1016" s="1" t="s">
-        <v>2309</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="1017" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1017" t="s">
-        <v>2083</v>
+        <v>2074</v>
       </c>
       <c r="B1017" t="s">
-        <v>2087</v>
+        <v>2078</v>
       </c>
       <c r="F1017" t="s">
-        <v>1942</v>
+        <v>2309</v>
       </c>
       <c r="J1017" s="1" t="s">
-        <v>2309</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="1018" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1018" t="s">
-        <v>2088</v>
+        <v>2079</v>
       </c>
       <c r="B1018" t="s">
-        <v>2089</v>
+        <v>2080</v>
       </c>
       <c r="F1018" t="s">
-        <v>1943</v>
+        <v>2310</v>
       </c>
       <c r="J1018" s="1" t="s">
-        <v>2310</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="1019" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1019" t="s">
-        <v>2090</v>
+        <v>2081</v>
       </c>
       <c r="B1019" t="s">
-        <v>2091</v>
+        <v>2082</v>
       </c>
       <c r="F1019" t="s">
-        <v>1943</v>
+        <v>2310</v>
       </c>
       <c r="J1019" s="1" t="s">
-        <v>2310</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="1020" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1020" t="s">
-        <v>2092</v>
+        <v>2083</v>
       </c>
       <c r="B1020" t="s">
-        <v>2093</v>
+        <v>2084</v>
       </c>
       <c r="F1020" t="s">
-        <v>1943</v>
+        <v>2310</v>
       </c>
       <c r="J1020" s="1" t="s">
-        <v>2310</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="1021" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1021" t="s">
-        <v>2094</v>
+        <v>2085</v>
       </c>
       <c r="B1021" t="s">
-        <v>2095</v>
+        <v>2086</v>
       </c>
       <c r="F1021" t="s">
-        <v>1943</v>
+        <v>2310</v>
       </c>
       <c r="J1021" s="1" t="s">
-        <v>2310</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="1022" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1022" t="s">
-        <v>2096</v>
+        <v>2087</v>
       </c>
       <c r="B1022" t="s">
-        <v>2097</v>
+        <v>2088</v>
       </c>
       <c r="F1022" t="s">
-        <v>1943</v>
+        <v>2310</v>
       </c>
       <c r="J1022" s="1" t="s">
-        <v>2310</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="1023" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1023" t="s">
-        <v>2098</v>
+        <v>2089</v>
       </c>
       <c r="B1023" t="s">
-        <v>2099</v>
+        <v>2090</v>
       </c>
       <c r="F1023" t="s">
-        <v>1943</v>
+        <v>2310</v>
       </c>
       <c r="J1023" s="1" t="s">
-        <v>2310</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="1024" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1024" t="s">
-        <v>2100</v>
+        <v>2091</v>
       </c>
       <c r="B1024" t="s">
-        <v>2101</v>
+        <v>2092</v>
       </c>
       <c r="F1024" t="s">
-        <v>1943</v>
+        <v>2310</v>
       </c>
       <c r="J1024" s="1" t="s">
-        <v>2310</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="1025" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1025" t="s">
-        <v>2102</v>
+        <v>2093</v>
       </c>
       <c r="B1025" t="s">
-        <v>2103</v>
+        <v>2094</v>
       </c>
       <c r="F1025" t="s">
-        <v>1943</v>
+        <v>2310</v>
       </c>
       <c r="J1025" s="1" t="s">
-        <v>2310</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="1026" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1026" t="s">
-        <v>2104</v>
+        <v>2095</v>
       </c>
       <c r="B1026" t="s">
-        <v>2105</v>
+        <v>2096</v>
       </c>
       <c r="F1026" t="s">
-        <v>1943</v>
+        <v>2310</v>
       </c>
       <c r="J1026" s="1" t="s">
-        <v>2310</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="1027" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1027" t="s">
-        <v>2106</v>
+        <v>2097</v>
       </c>
       <c r="B1027" t="s">
-        <v>2107</v>
+        <v>2098</v>
       </c>
       <c r="F1027" t="s">
-        <v>1943</v>
+        <v>2310</v>
       </c>
       <c r="J1027" s="1" t="s">
-        <v>2310</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="1028" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1028" t="s">
-        <v>2108</v>
+        <v>2099</v>
       </c>
       <c r="B1028" t="s">
-        <v>2109</v>
+        <v>2100</v>
       </c>
       <c r="F1028" t="s">
-        <v>1943</v>
+        <v>2310</v>
       </c>
       <c r="J1028" s="1" t="s">
-        <v>2310</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="1029" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1029" t="s">
-        <v>2022</v>
+        <v>2013</v>
       </c>
       <c r="B1029" t="s">
-        <v>2023</v>
+        <v>2014</v>
       </c>
       <c r="F1029" t="s">
-        <v>1943</v>
+        <v>2310</v>
       </c>
       <c r="J1029" s="1" t="s">
-        <v>2310</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="1030" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1030" t="s">
-        <v>2110</v>
+        <v>2101</v>
       </c>
       <c r="B1030" t="s">
-        <v>2111</v>
+        <v>2102</v>
       </c>
       <c r="F1030" t="s">
-        <v>1943</v>
+        <v>2310</v>
       </c>
       <c r="J1030" s="1" t="s">
-        <v>2310</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="1031" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1031" t="s">
-        <v>2112</v>
+        <v>2103</v>
       </c>
       <c r="B1031" t="s">
-        <v>2113</v>
+        <v>2104</v>
       </c>
       <c r="F1031" t="s">
-        <v>1943</v>
+        <v>2310</v>
       </c>
       <c r="J1031" s="1" t="s">
-        <v>2310</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="1032" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1032" t="s">
-        <v>2114</v>
+        <v>2105</v>
       </c>
       <c r="B1032" t="s">
-        <v>2115</v>
+        <v>2106</v>
       </c>
       <c r="F1032" t="s">
-        <v>1943</v>
+        <v>2310</v>
       </c>
       <c r="J1032" s="1" t="s">
-        <v>2310</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="1033" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1033" t="s">
-        <v>2116</v>
+        <v>2107</v>
       </c>
       <c r="B1033" t="s">
-        <v>2117</v>
+        <v>2108</v>
       </c>
       <c r="F1033" t="s">
-        <v>1943</v>
+        <v>2310</v>
       </c>
       <c r="J1033" s="1" t="s">
-        <v>2310</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="1034" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1034" t="s">
-        <v>2118</v>
+        <v>2109</v>
       </c>
       <c r="B1034" t="s">
-        <v>2119</v>
+        <v>2110</v>
       </c>
       <c r="F1034" t="s">
-        <v>1943</v>
+        <v>2310</v>
       </c>
       <c r="J1034" s="1" t="s">
-        <v>2310</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="1035" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1035" t="s">
-        <v>2120</v>
+        <v>2111</v>
       </c>
       <c r="B1035" t="s">
-        <v>2121</v>
+        <v>2112</v>
       </c>
       <c r="F1035" t="s">
-        <v>1943</v>
+        <v>2310</v>
       </c>
       <c r="J1035" s="1" t="s">
-        <v>2310</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="1036" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1036" t="s">
-        <v>2122</v>
+        <v>2113</v>
       </c>
       <c r="B1036" t="s">
-        <v>2123</v>
+        <v>2114</v>
       </c>
       <c r="F1036" t="s">
-        <v>1943</v>
+        <v>2310</v>
       </c>
       <c r="J1036" s="1" t="s">
-        <v>2310</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="1037" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1037" t="s">
-        <v>2124</v>
+        <v>2115</v>
       </c>
       <c r="B1037" t="s">
-        <v>2125</v>
+        <v>2116</v>
       </c>
       <c r="F1037" t="s">
-        <v>1943</v>
+        <v>2310</v>
       </c>
       <c r="J1037" s="1" t="s">
-        <v>2310</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="1038" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1038" t="s">
-        <v>2126</v>
+        <v>2117</v>
       </c>
       <c r="B1038" t="s">
-        <v>2127</v>
+        <v>2118</v>
       </c>
       <c r="F1038" t="s">
-        <v>1943</v>
+        <v>2310</v>
       </c>
       <c r="J1038" s="1" t="s">
-        <v>2310</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="1039" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1039" t="s">
-        <v>2128</v>
+        <v>2119</v>
       </c>
       <c r="B1039" t="s">
-        <v>2129</v>
+        <v>2120</v>
       </c>
       <c r="F1039" t="s">
-        <v>1943</v>
+        <v>2310</v>
       </c>
       <c r="J1039" s="1" t="s">
-        <v>2310</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="1040" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1040" t="s">
-        <v>2130</v>
+        <v>2121</v>
       </c>
       <c r="B1040" t="s">
-        <v>2131</v>
+        <v>2122</v>
       </c>
       <c r="F1040" t="s">
-        <v>1943</v>
+        <v>2310</v>
       </c>
       <c r="J1040" s="1" t="s">
-        <v>2310</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="1041" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1041" t="s">
-        <v>2132</v>
+        <v>2123</v>
       </c>
       <c r="B1041" t="s">
-        <v>2133</v>
+        <v>2124</v>
       </c>
       <c r="F1041" t="s">
-        <v>1943</v>
+        <v>2310</v>
       </c>
       <c r="J1041" s="1" t="s">
-        <v>2310</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="1042" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1042" t="s">
-        <v>2134</v>
+        <v>2125</v>
       </c>
       <c r="B1042" t="s">
-        <v>2135</v>
+        <v>2126</v>
       </c>
       <c r="F1042" t="s">
-        <v>1943</v>
+        <v>2310</v>
       </c>
       <c r="J1042" s="1" t="s">
-        <v>2310</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="1043" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1043" t="s">
-        <v>2136</v>
+        <v>2127</v>
       </c>
       <c r="B1043" t="s">
-        <v>2137</v>
+        <v>2128</v>
       </c>
       <c r="F1043" t="s">
-        <v>1943</v>
+        <v>2310</v>
       </c>
       <c r="J1043" s="1" t="s">
-        <v>2310</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="1044" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1044" t="s">
-        <v>2138</v>
+        <v>2129</v>
       </c>
       <c r="B1044" t="s">
-        <v>2139</v>
+        <v>2130</v>
       </c>
       <c r="F1044" t="s">
-        <v>1943</v>
+        <v>2310</v>
       </c>
       <c r="J1044" s="1" t="s">
-        <v>2310</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="1045" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1045" t="s">
-        <v>2140</v>
+        <v>2131</v>
       </c>
       <c r="B1045" t="s">
-        <v>2141</v>
+        <v>2132</v>
       </c>
       <c r="F1045" t="s">
-        <v>1943</v>
+        <v>2310</v>
       </c>
       <c r="J1045" s="1" t="s">
-        <v>2310</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="1046" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1046" t="s">
-        <v>2142</v>
+        <v>2133</v>
       </c>
       <c r="B1046" t="s">
-        <v>2143</v>
+        <v>2134</v>
       </c>
       <c r="F1046" t="s">
-        <v>1943</v>
+        <v>2310</v>
       </c>
       <c r="J1046" s="1" t="s">
-        <v>2310</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="1047" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1047" t="s">
-        <v>2144</v>
+        <v>2135</v>
       </c>
       <c r="B1047" t="s">
-        <v>2145</v>
+        <v>2136</v>
       </c>
       <c r="F1047" t="s">
-        <v>1943</v>
+        <v>2310</v>
       </c>
       <c r="J1047" s="1" t="s">
-        <v>2310</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="1048" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1048" t="s">
-        <v>2146</v>
+        <v>2137</v>
       </c>
       <c r="B1048" t="s">
-        <v>2147</v>
+        <v>2138</v>
       </c>
       <c r="F1048" t="s">
-        <v>1943</v>
+        <v>2310</v>
       </c>
       <c r="J1048" s="1" t="s">
-        <v>2310</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="1049" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1049" t="s">
-        <v>2148</v>
+        <v>2139</v>
       </c>
       <c r="B1049" t="s">
-        <v>2150</v>
+        <v>2141</v>
       </c>
       <c r="F1049" t="s">
-        <v>1943</v>
+        <v>2310</v>
       </c>
       <c r="J1049" s="1" t="s">
-        <v>2310</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="1050" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1050" t="s">
-        <v>2151</v>
+        <v>2142</v>
       </c>
       <c r="B1050" t="s">
-        <v>2152</v>
+        <v>2143</v>
       </c>
       <c r="F1050" t="s">
-        <v>1943</v>
+        <v>2310</v>
       </c>
       <c r="J1050" s="1" t="s">
-        <v>2310</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="1051" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1051" t="s">
-        <v>2153</v>
+        <v>2144</v>
       </c>
       <c r="B1051" t="s">
-        <v>2149</v>
+        <v>2140</v>
       </c>
       <c r="F1051" t="s">
-        <v>1943</v>
+        <v>2310</v>
       </c>
       <c r="J1051" s="1" t="s">
-        <v>2310</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="1052" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1052" t="s">
-        <v>2154</v>
+        <v>2145</v>
       </c>
       <c r="B1052" t="s">
-        <v>2155</v>
+        <v>2146</v>
       </c>
       <c r="F1052" t="s">
-        <v>1943</v>
+        <v>2310</v>
       </c>
       <c r="J1052" s="1" t="s">
-        <v>2310</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="1053" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1053" t="s">
-        <v>2156</v>
+        <v>2147</v>
       </c>
       <c r="B1053" t="s">
-        <v>2157</v>
+        <v>2148</v>
       </c>
       <c r="F1053" t="s">
-        <v>1943</v>
+        <v>2310</v>
       </c>
       <c r="J1053" s="1" t="s">
-        <v>2310</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="1054" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1054" t="s">
-        <v>2158</v>
+        <v>2149</v>
       </c>
       <c r="B1054" t="s">
-        <v>2159</v>
+        <v>2150</v>
       </c>
       <c r="F1054" t="s">
-        <v>1943</v>
+        <v>2310</v>
       </c>
       <c r="J1054" s="1" t="s">
-        <v>2310</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="1055" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1055" t="s">
-        <v>2160</v>
+        <v>2151</v>
       </c>
       <c r="B1055" t="s">
-        <v>2161</v>
+        <v>2152</v>
       </c>
       <c r="F1055" t="s">
-        <v>1943</v>
+        <v>2310</v>
       </c>
       <c r="J1055" s="1" t="s">
-        <v>2310</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="1056" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1056" t="s">
-        <v>2162</v>
+        <v>2153</v>
       </c>
       <c r="B1056" t="s">
-        <v>2163</v>
+        <v>2154</v>
       </c>
       <c r="F1056" t="s">
-        <v>1943</v>
+        <v>2310</v>
       </c>
       <c r="J1056" s="1" t="s">
-        <v>2310</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="1057" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1057" t="s">
-        <v>2164</v>
+        <v>2155</v>
       </c>
       <c r="B1057" t="s">
-        <v>2165</v>
+        <v>2156</v>
       </c>
       <c r="F1057" t="s">
-        <v>1943</v>
+        <v>2310</v>
       </c>
       <c r="J1057" s="1" t="s">
-        <v>2310</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="1058" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1058" t="s">
-        <v>2166</v>
+        <v>2157</v>
       </c>
       <c r="B1058" t="s">
-        <v>2167</v>
+        <v>2158</v>
       </c>
       <c r="F1058" t="s">
-        <v>1943</v>
+        <v>2310</v>
       </c>
       <c r="J1058" s="1" t="s">
-        <v>2310</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="1059" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1059" t="s">
-        <v>2168</v>
+        <v>2159</v>
       </c>
       <c r="B1059" t="s">
-        <v>2169</v>
+        <v>2160</v>
       </c>
       <c r="F1059" t="s">
-        <v>1943</v>
+        <v>2310</v>
       </c>
       <c r="J1059" s="1" t="s">
-        <v>2310</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="1060" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1060" t="s">
-        <v>2170</v>
+        <v>2161</v>
       </c>
       <c r="B1060" t="s">
-        <v>2171</v>
+        <v>2162</v>
       </c>
       <c r="F1060" t="s">
-        <v>1944</v>
+        <v>2311</v>
       </c>
       <c r="J1060" t="s">
-        <v>2311</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="1061" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1061" t="s">
-        <v>2172</v>
+        <v>2163</v>
       </c>
       <c r="B1061" t="s">
-        <v>2173</v>
+        <v>2164</v>
       </c>
       <c r="F1061" t="s">
-        <v>1944</v>
+        <v>2311</v>
       </c>
       <c r="J1061" t="s">
-        <v>2311</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="1062" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1062" t="s">
-        <v>2174</v>
+        <v>2165</v>
       </c>
       <c r="B1062" t="s">
-        <v>2175</v>
+        <v>2166</v>
       </c>
       <c r="F1062" t="s">
-        <v>1944</v>
+        <v>2311</v>
       </c>
       <c r="J1062" t="s">
-        <v>2311</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="1063" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1063" t="s">
-        <v>2176</v>
+        <v>2167</v>
       </c>
       <c r="B1063" t="s">
-        <v>2177</v>
+        <v>2168</v>
       </c>
       <c r="F1063" t="s">
-        <v>1944</v>
+        <v>2311</v>
       </c>
       <c r="J1063" t="s">
-        <v>2311</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="1064" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1064" t="s">
-        <v>2178</v>
+        <v>2169</v>
       </c>
       <c r="B1064" t="s">
-        <v>2179</v>
+        <v>2170</v>
       </c>
       <c r="F1064" t="s">
-        <v>1944</v>
+        <v>2311</v>
       </c>
       <c r="J1064" t="s">
-        <v>2311</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="1065" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1065" t="s">
-        <v>2180</v>
+        <v>2171</v>
       </c>
       <c r="B1065" t="s">
-        <v>2181</v>
+        <v>2172</v>
       </c>
       <c r="F1065" t="s">
-        <v>1944</v>
+        <v>2311</v>
       </c>
       <c r="J1065" t="s">
-        <v>2311</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="1066" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1066" t="s">
-        <v>2182</v>
+        <v>2173</v>
       </c>
       <c r="B1066" t="s">
-        <v>2183</v>
+        <v>2174</v>
       </c>
       <c r="F1066" t="s">
-        <v>1944</v>
+        <v>2311</v>
       </c>
       <c r="J1066" t="s">
-        <v>2311</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="1067" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1067" t="s">
-        <v>2184</v>
+        <v>2175</v>
       </c>
       <c r="B1067" t="s">
-        <v>2185</v>
+        <v>2176</v>
       </c>
       <c r="F1067" t="s">
-        <v>1944</v>
+        <v>2311</v>
       </c>
       <c r="J1067" t="s">
-        <v>2311</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="1068" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1068" t="s">
-        <v>2186</v>
+        <v>2177</v>
       </c>
       <c r="B1068" t="s">
-        <v>2187</v>
+        <v>2178</v>
       </c>
       <c r="F1068" t="s">
-        <v>1944</v>
+        <v>2311</v>
       </c>
       <c r="J1068" t="s">
-        <v>2311</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="1069" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1069" t="s">
-        <v>2188</v>
+        <v>2179</v>
       </c>
       <c r="B1069" t="s">
-        <v>2189</v>
+        <v>2180</v>
       </c>
       <c r="F1069" t="s">
-        <v>1944</v>
+        <v>2311</v>
       </c>
       <c r="J1069" t="s">
-        <v>2311</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="1070" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1070" t="s">
-        <v>2190</v>
+        <v>2181</v>
       </c>
       <c r="B1070" t="s">
-        <v>2191</v>
+        <v>2182</v>
       </c>
       <c r="F1070" t="s">
-        <v>1944</v>
+        <v>2311</v>
       </c>
       <c r="J1070" t="s">
-        <v>2311</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="1071" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1071" t="s">
-        <v>2192</v>
+        <v>2183</v>
       </c>
       <c r="B1071" t="s">
-        <v>2193</v>
+        <v>2184</v>
       </c>
       <c r="F1071" t="s">
-        <v>1944</v>
+        <v>2311</v>
       </c>
       <c r="J1071" t="s">
-        <v>2311</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="1072" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1072" t="s">
-        <v>2194</v>
+        <v>2185</v>
       </c>
       <c r="B1072" t="s">
-        <v>2195</v>
+        <v>2186</v>
       </c>
       <c r="F1072" t="s">
-        <v>1944</v>
+        <v>2311</v>
       </c>
       <c r="J1072" t="s">
-        <v>2311</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="1073" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1073" t="s">
-        <v>2196</v>
+        <v>2187</v>
       </c>
       <c r="B1073" t="s">
-        <v>2197</v>
+        <v>2188</v>
       </c>
       <c r="F1073" t="s">
-        <v>1944</v>
+        <v>2311</v>
       </c>
       <c r="J1073" t="s">
-        <v>2311</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="1074" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1074" t="s">
-        <v>2198</v>
+        <v>2189</v>
       </c>
       <c r="B1074" t="s">
-        <v>2199</v>
+        <v>2190</v>
       </c>
       <c r="F1074" t="s">
-        <v>1944</v>
+        <v>2311</v>
       </c>
       <c r="J1074" t="s">
-        <v>2311</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="1075" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1075" t="s">
-        <v>2200</v>
+        <v>2191</v>
       </c>
       <c r="B1075" t="s">
-        <v>2201</v>
+        <v>2192</v>
       </c>
       <c r="F1075" t="s">
-        <v>1944</v>
+        <v>2311</v>
       </c>
       <c r="J1075" t="s">
-        <v>2311</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="1076" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1076" t="s">
-        <v>2202</v>
+        <v>2193</v>
       </c>
       <c r="B1076" t="s">
-        <v>2203</v>
+        <v>2194</v>
       </c>
       <c r="F1076" t="s">
-        <v>1944</v>
+        <v>2311</v>
       </c>
       <c r="J1076" t="s">
-        <v>2311</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="1077" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1077" t="s">
-        <v>2204</v>
+        <v>2195</v>
       </c>
       <c r="B1077" t="s">
-        <v>2205</v>
+        <v>2196</v>
       </c>
       <c r="F1077" t="s">
-        <v>1944</v>
+        <v>2311</v>
       </c>
       <c r="J1077" t="s">
-        <v>2311</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="1078" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1078" t="s">
-        <v>2206</v>
+        <v>2197</v>
       </c>
       <c r="B1078" t="s">
-        <v>2207</v>
+        <v>2198</v>
       </c>
       <c r="F1078" t="s">
-        <v>1944</v>
+        <v>2311</v>
       </c>
       <c r="J1078" t="s">
-        <v>2311</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="1079" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1079" t="s">
-        <v>2208</v>
+        <v>2199</v>
       </c>
       <c r="B1079" t="s">
-        <v>2209</v>
+        <v>2200</v>
       </c>
       <c r="F1079" t="s">
-        <v>1944</v>
+        <v>2311</v>
       </c>
       <c r="J1079" t="s">
-        <v>2311</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="1080" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1080" t="s">
-        <v>2210</v>
+        <v>2201</v>
       </c>
       <c r="B1080" t="s">
-        <v>2211</v>
+        <v>2202</v>
       </c>
       <c r="F1080" t="s">
-        <v>1944</v>
+        <v>2311</v>
       </c>
       <c r="J1080" t="s">
-        <v>2311</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="1081" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1081" t="s">
-        <v>2212</v>
+        <v>2203</v>
       </c>
       <c r="B1081" t="s">
-        <v>2213</v>
+        <v>2204</v>
       </c>
       <c r="F1081" t="s">
-        <v>1944</v>
+        <v>2311</v>
       </c>
       <c r="J1081" t="s">
-        <v>2311</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="1082" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1082" t="s">
-        <v>2214</v>
+        <v>2205</v>
       </c>
       <c r="B1082" t="s">
-        <v>2215</v>
+        <v>2206</v>
       </c>
       <c r="F1082" t="s">
-        <v>1944</v>
+        <v>2311</v>
       </c>
       <c r="J1082" t="s">
-        <v>2311</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="1083" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1083" t="s">
-        <v>2216</v>
+        <v>2207</v>
       </c>
       <c r="B1083" t="s">
-        <v>2217</v>
+        <v>2208</v>
       </c>
       <c r="F1083" t="s">
-        <v>1944</v>
+        <v>2311</v>
       </c>
       <c r="J1083" t="s">
-        <v>2311</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="1084" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1084" t="s">
-        <v>2218</v>
+        <v>2209</v>
       </c>
       <c r="B1084" t="s">
-        <v>2219</v>
+        <v>2210</v>
       </c>
       <c r="F1084" t="s">
-        <v>1944</v>
+        <v>2311</v>
       </c>
       <c r="J1084" t="s">
-        <v>2311</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="1085" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1085" t="s">
-        <v>2220</v>
+        <v>2211</v>
       </c>
       <c r="B1085" t="s">
-        <v>2221</v>
+        <v>2212</v>
       </c>
       <c r="F1085" t="s">
-        <v>1944</v>
+        <v>2311</v>
       </c>
       <c r="J1085" t="s">
-        <v>2311</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="1086" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1086" t="s">
-        <v>2222</v>
+        <v>2213</v>
       </c>
       <c r="B1086" t="s">
-        <v>2223</v>
+        <v>2214</v>
       </c>
       <c r="F1086" t="s">
-        <v>1944</v>
+        <v>2311</v>
       </c>
       <c r="J1086" t="s">
-        <v>2311</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="1087" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1087" t="s">
-        <v>2224</v>
+        <v>2215</v>
       </c>
       <c r="B1087" t="s">
-        <v>2225</v>
+        <v>2216</v>
       </c>
       <c r="F1087" t="s">
-        <v>1944</v>
+        <v>2311</v>
       </c>
       <c r="J1087" t="s">
-        <v>2311</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="1088" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1088" t="s">
-        <v>2226</v>
+        <v>2217</v>
       </c>
       <c r="B1088" t="s">
-        <v>2233</v>
+        <v>2224</v>
       </c>
       <c r="F1088" t="s">
-        <v>1945</v>
+        <v>2312</v>
       </c>
       <c r="J1088" t="s">
-        <v>2312</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="1089" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1089" t="s">
-        <v>2227</v>
+        <v>2218</v>
       </c>
       <c r="B1089" t="s">
-        <v>2234</v>
+        <v>2225</v>
       </c>
       <c r="F1089" t="s">
-        <v>1945</v>
+        <v>2312</v>
       </c>
       <c r="J1089" t="s">
-        <v>2312</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="1090" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1090" t="s">
-        <v>2228</v>
+        <v>2219</v>
       </c>
       <c r="B1090" t="s">
-        <v>2235</v>
+        <v>2226</v>
       </c>
       <c r="F1090" t="s">
-        <v>1945</v>
+        <v>2312</v>
       </c>
       <c r="J1090" t="s">
-        <v>2312</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="1091" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1091" t="s">
-        <v>2229</v>
+        <v>2220</v>
       </c>
       <c r="B1091" t="s">
-        <v>2236</v>
+        <v>2227</v>
       </c>
       <c r="F1091" t="s">
-        <v>1945</v>
+        <v>2312</v>
       </c>
       <c r="J1091" t="s">
-        <v>2312</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="1092" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1092" t="s">
-        <v>2230</v>
+        <v>2221</v>
       </c>
       <c r="B1092" t="s">
-        <v>2236</v>
+        <v>2227</v>
       </c>
       <c r="F1092" t="s">
-        <v>1945</v>
+        <v>2312</v>
       </c>
       <c r="J1092" t="s">
-        <v>2312</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="1093" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1093" t="s">
-        <v>2231</v>
+        <v>2222</v>
       </c>
       <c r="B1093" t="s">
-        <v>2237</v>
+        <v>2228</v>
       </c>
       <c r="F1093" t="s">
-        <v>1945</v>
+        <v>2312</v>
       </c>
       <c r="J1093" t="s">
-        <v>2312</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="1094" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1094" t="s">
-        <v>2232</v>
+        <v>2223</v>
       </c>
       <c r="B1094" t="s">
-        <v>2238</v>
+        <v>2229</v>
       </c>
       <c r="F1094" t="s">
-        <v>1945</v>
+        <v>2312</v>
       </c>
       <c r="J1094" t="s">
-        <v>2312</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="1095" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1095" t="s">
-        <v>2102</v>
+        <v>2093</v>
       </c>
       <c r="B1095" t="s">
-        <v>2103</v>
+        <v>2094</v>
       </c>
       <c r="F1095" t="s">
-        <v>1945</v>
+        <v>2312</v>
       </c>
       <c r="J1095" t="s">
-        <v>2312</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="1096" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1096" t="s">
-        <v>2239</v>
+        <v>2230</v>
       </c>
       <c r="B1096" t="s">
-        <v>2240</v>
+        <v>2231</v>
       </c>
       <c r="F1096" t="s">
-        <v>1945</v>
+        <v>2312</v>
       </c>
       <c r="J1096" t="s">
-        <v>2312</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="1097" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1097" t="s">
-        <v>2241</v>
+        <v>2232</v>
       </c>
       <c r="B1097" t="s">
-        <v>2242</v>
+        <v>2233</v>
       </c>
       <c r="F1097" t="s">
-        <v>1945</v>
+        <v>2312</v>
       </c>
       <c r="J1097" t="s">
-        <v>2312</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="1098" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1098" t="s">
-        <v>2243</v>
+        <v>2234</v>
       </c>
       <c r="B1098" t="s">
-        <v>2244</v>
+        <v>2235</v>
       </c>
       <c r="F1098" t="s">
-        <v>1945</v>
+        <v>2312</v>
       </c>
       <c r="J1098" t="s">
-        <v>2312</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="1099" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1099" t="s">
-        <v>2245</v>
+        <v>2236</v>
       </c>
       <c r="B1099" t="s">
-        <v>2246</v>
+        <v>2237</v>
       </c>
       <c r="F1099" t="s">
-        <v>1945</v>
+        <v>2312</v>
       </c>
       <c r="J1099" t="s">
-        <v>2312</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="1100" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1100" t="s">
-        <v>2247</v>
+        <v>2238</v>
       </c>
       <c r="B1100" t="s">
-        <v>2248</v>
+        <v>2239</v>
       </c>
       <c r="F1100" t="s">
-        <v>1945</v>
+        <v>2312</v>
       </c>
       <c r="J1100" t="s">
-        <v>2312</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="1101" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1101" t="s">
-        <v>2249</v>
+        <v>2240</v>
       </c>
       <c r="B1101" t="s">
-        <v>2250</v>
+        <v>2241</v>
       </c>
       <c r="F1101" t="s">
-        <v>1945</v>
+        <v>2312</v>
       </c>
       <c r="J1101" t="s">
-        <v>2312</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="1102" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1102" t="s">
-        <v>2251</v>
+        <v>2242</v>
       </c>
       <c r="B1102" t="s">
-        <v>2252</v>
+        <v>2243</v>
       </c>
       <c r="F1102" t="s">
-        <v>1945</v>
+        <v>2312</v>
       </c>
       <c r="J1102" t="s">
-        <v>2312</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="1103" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1103" t="s">
-        <v>2253</v>
+        <v>2244</v>
       </c>
       <c r="B1103" t="s">
-        <v>2254</v>
+        <v>2245</v>
       </c>
       <c r="F1103" t="s">
-        <v>1945</v>
+        <v>2312</v>
       </c>
       <c r="J1103" t="s">
-        <v>2312</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="1104" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1104" t="s">
-        <v>2255</v>
+        <v>2246</v>
       </c>
       <c r="B1104" t="s">
-        <v>2256</v>
+        <v>2247</v>
       </c>
       <c r="F1104" t="s">
-        <v>1945</v>
+        <v>2312</v>
       </c>
       <c r="J1104" t="s">
-        <v>2312</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="1105" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1105" t="s">
-        <v>2257</v>
+        <v>2248</v>
       </c>
       <c r="B1105" t="s">
-        <v>2258</v>
+        <v>2249</v>
       </c>
       <c r="F1105" t="s">
-        <v>1945</v>
+        <v>2312</v>
       </c>
       <c r="J1105" t="s">
-        <v>2312</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="1106" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1106" t="s">
-        <v>2259</v>
+        <v>2250</v>
       </c>
       <c r="B1106" t="s">
-        <v>2260</v>
+        <v>2251</v>
       </c>
       <c r="F1106" t="s">
-        <v>1945</v>
+        <v>2312</v>
       </c>
       <c r="J1106" t="s">
-        <v>2312</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="1107" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1107" t="s">
-        <v>2261</v>
+        <v>2252</v>
       </c>
       <c r="B1107" t="s">
-        <v>2262</v>
+        <v>2253</v>
       </c>
       <c r="F1107" t="s">
-        <v>1945</v>
+        <v>2312</v>
       </c>
       <c r="J1107" t="s">
-        <v>2312</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="1108" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1108" t="s">
-        <v>2263</v>
+        <v>2254</v>
       </c>
       <c r="B1108" t="s">
-        <v>2264</v>
+        <v>2255</v>
       </c>
       <c r="F1108" t="s">
-        <v>1945</v>
+        <v>2312</v>
       </c>
       <c r="J1108" t="s">
-        <v>2312</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="1109" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1109" t="s">
-        <v>2265</v>
+        <v>2256</v>
       </c>
       <c r="B1109" t="s">
-        <v>2266</v>
+        <v>2257</v>
       </c>
       <c r="F1109" t="s">
-        <v>1945</v>
+        <v>2312</v>
       </c>
       <c r="J1109" t="s">
-        <v>2312</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="1110" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1110" t="s">
-        <v>2268</v>
+        <v>2259</v>
       </c>
       <c r="B1110" t="s">
-        <v>2267</v>
+        <v>2258</v>
       </c>
       <c r="F1110" t="s">
-        <v>1945</v>
+        <v>2312</v>
       </c>
       <c r="J1110" t="s">
-        <v>2312</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="1111" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1111" t="s">
-        <v>2269</v>
+        <v>2260</v>
       </c>
       <c r="B1111" t="s">
-        <v>2270</v>
+        <v>2261</v>
       </c>
       <c r="F1111" t="s">
-        <v>1945</v>
+        <v>2312</v>
       </c>
       <c r="J1111" t="s">
-        <v>2312</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="1112" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1112" t="s">
-        <v>2271</v>
+        <v>2262</v>
       </c>
       <c r="B1112" s="1" t="s">
-        <v>2272</v>
+        <v>2263</v>
       </c>
       <c r="F1112" t="s">
-        <v>1945</v>
+        <v>2312</v>
       </c>
       <c r="J1112" t="s">
-        <v>2312</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="1113" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1113" t="s">
-        <v>2273</v>
+        <v>2264</v>
       </c>
       <c r="B1113" t="s">
-        <v>2274</v>
+        <v>2265</v>
       </c>
       <c r="F1113" t="s">
-        <v>1945</v>
+        <v>2312</v>
       </c>
       <c r="J1113" t="s">
-        <v>2312</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="1114" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1114" t="s">
-        <v>2275</v>
+        <v>2266</v>
       </c>
       <c r="B1114" t="s">
-        <v>2276</v>
+        <v>2267</v>
       </c>
       <c r="F1114" t="s">
-        <v>1945</v>
+        <v>2312</v>
       </c>
       <c r="J1114" t="s">
-        <v>2312</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="1115" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1115" t="s">
-        <v>2277</v>
+        <v>2268</v>
       </c>
       <c r="B1115" t="s">
-        <v>2278</v>
+        <v>2269</v>
       </c>
       <c r="F1115" t="s">
-        <v>1945</v>
+        <v>2312</v>
       </c>
       <c r="J1115" t="s">
-        <v>2312</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="1116" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1116" t="s">
-        <v>2279</v>
+        <v>2270</v>
       </c>
       <c r="B1116" s="1" t="s">
-        <v>2280</v>
+        <v>2271</v>
       </c>
       <c r="F1116" t="s">
-        <v>1945</v>
+        <v>2312</v>
       </c>
       <c r="J1116" t="s">
-        <v>2312</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="1117" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1117" t="s">
-        <v>2281</v>
+        <v>2272</v>
       </c>
       <c r="B1117" t="s">
-        <v>2282</v>
+        <v>2273</v>
       </c>
       <c r="F1117" t="s">
-        <v>1945</v>
+        <v>2312</v>
       </c>
       <c r="J1117" t="s">
-        <v>2312</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="1118" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1118" t="s">
-        <v>2283</v>
+        <v>2274</v>
       </c>
       <c r="B1118" t="s">
-        <v>2284</v>
+        <v>2275</v>
       </c>
       <c r="F1118" t="s">
-        <v>1945</v>
+        <v>2312</v>
       </c>
       <c r="J1118" t="s">
-        <v>2312</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="1119" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1119" t="s">
-        <v>2285</v>
+        <v>2276</v>
       </c>
       <c r="B1119" t="s">
-        <v>2286</v>
+        <v>2277</v>
       </c>
       <c r="F1119" t="s">
-        <v>1945</v>
+        <v>2312</v>
       </c>
       <c r="J1119" t="s">
-        <v>2312</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="1120" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1120" t="s">
-        <v>2287</v>
+        <v>2278</v>
       </c>
       <c r="B1120" t="s">
-        <v>2288</v>
+        <v>2279</v>
       </c>
       <c r="F1120" t="s">
-        <v>1945</v>
+        <v>2312</v>
       </c>
       <c r="J1120" t="s">
-        <v>2312</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="1121" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1121" t="s">
-        <v>2289</v>
+        <v>2280</v>
       </c>
       <c r="B1121" t="s">
-        <v>2290</v>
+        <v>2281</v>
       </c>
       <c r="F1121" t="s">
-        <v>1945</v>
+        <v>2312</v>
       </c>
       <c r="J1121" t="s">
-        <v>2312</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="1122" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1122" t="s">
-        <v>2291</v>
+        <v>2282</v>
       </c>
       <c r="B1122" t="s">
-        <v>2292</v>
+        <v>2283</v>
       </c>
       <c r="F1122" t="s">
-        <v>1946</v>
+        <v>2313</v>
       </c>
       <c r="J1122" t="s">
-        <v>2313</v>
+        <v>2304</v>
       </c>
     </row>
     <row r="1123" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1123" t="s">
-        <v>2293</v>
+        <v>2284</v>
       </c>
       <c r="B1123" t="s">
-        <v>2294</v>
+        <v>2285</v>
       </c>
       <c r="F1123" t="s">
-        <v>1947</v>
+        <v>2314</v>
       </c>
       <c r="J1123" t="s">
-        <v>2314</v>
+        <v>2305</v>
       </c>
     </row>
     <row r="1124" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1124" t="s">
-        <v>2296</v>
+        <v>2287</v>
       </c>
       <c r="B1124" t="s">
-        <v>2295</v>
+        <v>2286</v>
       </c>
       <c r="F1124" t="s">
-        <v>1947</v>
+        <v>2314</v>
       </c>
       <c r="J1124" t="s">
-        <v>2314</v>
+        <v>2305</v>
       </c>
     </row>
     <row r="1125" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1125" t="s">
-        <v>2298</v>
+        <v>2289</v>
       </c>
       <c r="B1125" t="s">
-        <v>2297</v>
+        <v>2288</v>
       </c>
       <c r="F1125" t="s">
-        <v>1947</v>
+        <v>2314</v>
       </c>
       <c r="J1125" t="s">
-        <v>2314</v>
+        <v>2305</v>
       </c>
     </row>
     <row r="1126" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1126" t="s">
-        <v>2299</v>
+        <v>2290</v>
       </c>
       <c r="B1126" t="s">
-        <v>2300</v>
+        <v>2291</v>
       </c>
       <c r="F1126" t="s">
-        <v>1947</v>
+        <v>2314</v>
       </c>
       <c r="J1126" t="s">
-        <v>2314</v>
+        <v>2305</v>
       </c>
     </row>
     <row r="1127" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1127" t="s">
-        <v>2302</v>
+        <v>2293</v>
       </c>
       <c r="B1127" t="s">
-        <v>2301</v>
+        <v>2292</v>
       </c>
       <c r="F1127" t="s">
-        <v>1947</v>
+        <v>2314</v>
       </c>
       <c r="J1127" t="s">
-        <v>2314</v>
+        <v>2305</v>
       </c>
     </row>
     <row r="1128" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1128" t="s">
-        <v>2303</v>
+        <v>2294</v>
       </c>
       <c r="B1128" t="s">
-        <v>2304</v>
+        <v>2295</v>
       </c>
       <c r="F1128" t="s">
-        <v>1947</v>
+        <v>2314</v>
       </c>
       <c r="J1128" t="s">
-        <v>2314</v>
+        <v>2305</v>
       </c>
     </row>
     <row r="1129" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1129" t="s">
+        <v>2296</v>
+      </c>
+      <c r="B1129" t="s">
+        <v>2297</v>
+      </c>
+      <c r="F1129" t="s">
+        <v>2314</v>
+      </c>
+      <c r="J1129" t="s">
         <v>2305</v>
-      </c>
-      <c r="B1129" t="s">
-        <v>2306</v>
-      </c>
-      <c r="F1129" t="s">
-        <v>1947</v>
-      </c>
-      <c r="J1129" t="s">
-        <v>2314</v>
       </c>
     </row>
   </sheetData>

</xml_diff>